<commit_message>
[FIX] in Stops Report use just Odometer as heading
</commit_message>
<xml_diff>
--- a/templates/export/stops.xlsx
+++ b/templates/export/stops.xlsx
@@ -69,7 +69,7 @@
     <t>Start Address</t>
   </si>
   <si>
-    <t>Start Odometer</t>
+    <t>Odometer</t>
   </si>
   <si>
     <t>End</t>
@@ -258,7 +258,7 @@
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="4" fillId="2" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment horizontal="center" shrinkToFit="0" wrapText="1"/>
+      <alignment horizontal="center" readingOrder="0" shrinkToFit="0" wrapText="1"/>
     </xf>
     <xf borderId="3" fillId="0" fontId="7" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="center" wrapText="1"/>

</xml_diff>